<commit_message>
Adicioado ordem de servico atualizada, email de aceite ao cliente e arquivo xlsx atualizado
</commit_message>
<xml_diff>
--- a/Documentacao/processo_grupo1.xlsx
+++ b/Documentacao/processo_grupo1.xlsx
@@ -40,7 +40,7 @@
     <t>1. Requerimento</t>
   </si>
   <si>
-    <t>1.1 Elicitação</t>
+    <t>1.1 Elicitar</t>
   </si>
   <si>
     <t>SIM</t>
@@ -55,7 +55,7 @@
     <t>Ordem de serviço</t>
   </si>
   <si>
-    <t>1.2 Documentação</t>
+    <t>1.2 Documentar</t>
   </si>
   <si>
     <t>1.1</t>
@@ -70,7 +70,7 @@
     <t>Especificação de requisitos</t>
   </si>
   <si>
-    <t>1.3 Validação Requisitos</t>
+    <t>1.3 Validar Requisito</t>
   </si>
   <si>
     <t>1.2</t>
@@ -82,7 +82,7 @@
     <t>2. Projeto</t>
   </si>
   <si>
-    <t xml:space="preserve">2.1 Design Arquitetura </t>
+    <t xml:space="preserve">2.1 Criar Design De Arquitetura </t>
   </si>
   <si>
     <t>1.3</t>
@@ -91,7 +91,7 @@
     <t>Baseline do Software, Documento de Classes</t>
   </si>
   <si>
-    <t>2.2 Projeto do BD</t>
+    <t>2.2 Projetar BD</t>
   </si>
   <si>
     <t>2.1</t>
@@ -106,7 +106,7 @@
     <t>3. Desenvolvimento</t>
   </si>
   <si>
-    <t>3.1 Codificação</t>
+    <t>3.1 Codificar</t>
   </si>
   <si>
     <t>2.2</t>
@@ -115,7 +115,7 @@
     <t>Código fonte</t>
   </si>
   <si>
-    <t>3.2 Teste</t>
+    <t>3.2 Testar</t>
   </si>
   <si>
     <t>3.1</t>
@@ -124,7 +124,7 @@
     <t xml:space="preserve">Casos de teste </t>
   </si>
   <si>
-    <t>3.3 Entrega</t>
+    <t>3.3 Entregar</t>
   </si>
   <si>
     <t>3.1 e 3.2</t>
@@ -659,7 +659,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>479425</xdr:colOff>
+      <xdr:colOff>263525</xdr:colOff>
       <xdr:row>58</xdr:row>
       <xdr:rowOff>83513</xdr:rowOff>
     </xdr:to>
@@ -1773,7 +1773,7 @@
   <sheetFormatPr defaultColWidth="11.8333" defaultRowHeight="12.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="21.1719" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.8516" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.6719" style="1" customWidth="1"/>
     <col min="3" max="4" width="15.6719" style="1" customWidth="1"/>
     <col min="5" max="5" width="20" style="1" customWidth="1"/>
     <col min="6" max="7" width="42.6719" style="1" customWidth="1"/>

</xml_diff>